<commit_message>
提交 Signed-off-by: hxy <1305149167@qq.com>
Signed-off-by: hxy <1305149167@qq.com>
</commit_message>
<xml_diff>
--- a/data/woniuboss4.0_case_huang.xlsx
+++ b/data/woniuboss4.0_case_huang.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IT\torgit\testing\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63E9D299-9818-4AB5-980C-8016259528F7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{136DB4C5-F610-461E-9D7E-D7D25CEEE413}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
@@ -272,9 +272,283 @@
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
-    <r>
-      <t>start_js=document.querySelector(\"#addcourse &gt; div.row &gt; div:nth-child(1) &gt; input\") end_js=document.querySelector(\"#modifyCourseForm &gt; div &gt; div &gt; div:nth-child(2) &gt; input\")
-start_time=2020-05-17
+    <t>alter-success</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>outcome=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">优
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>evaluate=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>善于表达</t>
+    </r>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>add_002</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>technical_interview_cases</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>do_add_interview_test</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>outcome=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">中
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>evaluate=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>基础知识不扎实</t>
+    </r>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>teacher_on_duty_cases</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>do_add_duty_test</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>alter_003</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>alter_004</t>
+  </si>
+  <si>
+    <t>do_alter_duty_test</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>alter-success</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>application_for_extra_work_cases</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>do_add_overtime_test</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>start_time=2020-05-10 09:30
+end_time=2020-05-10 18:30
+accounting=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="微软雅黑"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">结算工资
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>hours=2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="微软雅黑"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">小时
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>region=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="微软雅黑"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>成都</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+reason=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="微软雅黑"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>出去旅游世界太大我想去看看</t>
+    </r>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>start_time=2020-05-20 08:30
+end_time=2020-05-20 20:30
+accounting=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="微软雅黑"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">结算工资
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>hours=8</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="微软雅黑"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">小时
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>region=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="微软雅黑"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>成都</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+reason=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="微软雅黑"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>回老家吃小龙虾校长要不要给你带点</t>
+    </r>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>start_time=2020-05-17
 end_time=2020-05-24
 teacher=</t>
     </r>
@@ -333,8 +607,7 @@
   </si>
   <si>
     <r>
-      <t>start_js=document.querySelector(\"#addcourse &gt; div.row &gt; div:nth-child(1) &gt; input\") end_js=document.querySelector(\"#modifyCourseForm &gt; div &gt; div &gt; div:nth-child(2) &gt; input\")
-start_time=2020-05-25
+      <t>start_time=2020-05-25
 end_time=2020-06-02
 teacher=</t>
     </r>
@@ -393,8 +666,7 @@
   </si>
   <si>
     <r>
-      <t>start_js=document.querySelector(\"#modifyCourseForm &gt; div &gt; div &gt; div:nth-child(1) &gt; input\") end_js=document.querySelector(\"#modifyCourseForm &gt; div &gt; div &gt; div:nth-child(2) &gt; input\")
-start_time=2020-05-25
+      <t>start_time=2020-05-25
 end_time=2020-06-02
 teacher=</t>
     </r>
@@ -490,13 +762,8 @@
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
-    <t>alter-success</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>start_js=document.querySelector(\"#modifyCourseForm &gt; div &gt; div &gt; div:nth-child(1) &gt; input\") end_js=document.querySelector(\"#modifyCourseForm &gt; div &gt; div &gt; div:nth-child(2) &gt; input\")
-start_time=2020-05-25
+    <r>
+      <t>start_time=2020-05-25
 end_time=2020-06-02
 teacher=</t>
     </r>
@@ -555,7 +822,7 @@
   </si>
   <si>
     <r>
-      <t>outcome=</t>
+      <t>teacher=</t>
     </r>
     <r>
       <rPr>
@@ -565,7 +832,7 @@
         <family val="2"/>
         <charset val="134"/>
       </rPr>
-      <t xml:space="preserve">优
+      <t xml:space="preserve">吴用
 </t>
     </r>
     <r>
@@ -575,7 +842,13 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>evaluate=</t>
+      <t>duty_time=2020-04-30</t>
+    </r>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>teacher=</t>
     </r>
     <r>
       <rPr>
@@ -585,25 +858,23 @@
         <family val="2"/>
         <charset val="134"/>
       </rPr>
-      <t>善于表达</t>
-    </r>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>add_002</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>technical_interview_cases</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>do_add_interview_test</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>outcome=</t>
+      <t xml:space="preserve">江鸟
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>duty_time=2020-03-11</t>
+    </r>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>teacher=</t>
     </r>
     <r>
       <rPr>
@@ -613,7 +884,7 @@
         <family val="2"/>
         <charset val="134"/>
       </rPr>
-      <t xml:space="preserve">中
+      <t xml:space="preserve">佛祖
 </t>
     </r>
     <r>
@@ -623,26 +894,8 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>evaluate=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t>基础知识不扎实</t>
-    </r>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>teacher_on_duty_cases</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>do_add_duty_test</t>
+      <t>duty_time=2020-05-21</t>
+    </r>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
@@ -667,268 +920,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>time_js=document.querySelector("#addDuty-table &gt; tr &gt; td:nth-child(2) &gt; input")
-duty_time=2020-05-20</t>
-    </r>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>teacher=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">佛祖
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>time_js=document.querySelector("#addDuty-table &gt; tr &gt; td:nth-child(2) &gt; input")
-duty_time=2020-05-21</t>
-    </r>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>alter_003</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>alter_004</t>
-  </si>
-  <si>
-    <t>do_alter_duty_test</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>alter-success</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>teacher=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">江鸟
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>time_js=document.querySelector("#addDuty-table &gt; tr &gt; td:nth-child(2) &gt; input")
-duty_time=2020-03-11</t>
-    </r>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>teacher=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">吴用
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>time_js=document.querySelector("#addDuty-table &gt; tr &gt; td:nth-child(2) &gt; input")
-duty_time=2020-04-30</t>
-    </r>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>application_for_extra_work_cases</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>do_add_overtime_test</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>start_time=2020-05-10 09:30
-end_time=2020-05-10 18:30
-accounting=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="微软雅黑"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">结算工资
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>hours=2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="微软雅黑"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">小时
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>region=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="微软雅黑"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t>成都</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-reason=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="微软雅黑"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t>出去旅游世界太大我想去看看</t>
-    </r>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>start_time=2020-05-20 08:30
-end_time=2020-05-20 20:30
-accounting=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="微软雅黑"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">结算工资
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>hours=8</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="微软雅黑"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">小时
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>region=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="微软雅黑"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t>成都</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-reason=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="微软雅黑"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t>回老家吃小龙虾校长要不要给你带点</t>
+      <t>duty_time=2020-05-20</t>
     </r>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
@@ -1540,8 +1532,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C2A6EE2-B6CB-4035-91E6-069CF874E712}">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1572,7 +1564,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="143.4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="88.2" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>20</v>
       </c>
@@ -1586,13 +1578,13 @@
         <v>27</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="143.4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="88.2" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>22</v>
       </c>
@@ -1606,7 +1598,7 @@
         <v>27</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="F3" s="7" t="s">
         <v>21</v>
@@ -1652,7 +1644,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="143.4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="88.2" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>31</v>
       </c>
@@ -1666,13 +1658,13 @@
         <v>33</v>
       </c>
       <c r="E6" s="14" t="s">
-        <v>36</v>
+        <v>52</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="143.4" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="88.2" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>32</v>
       </c>
@@ -1686,10 +1678,10 @@
         <v>33</v>
       </c>
       <c r="E7" s="14" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -1704,7 +1696,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:F3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1741,16 +1733,16 @@
         <v>20</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>21</v>
@@ -1758,19 +1750,19 @@
     </row>
     <row r="3" spans="1:6" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>21</v>
@@ -1788,7 +1780,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1820,84 +1812,84 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="42" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="28.2" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>20</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="42" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="28.2" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="B3" s="9" t="s">
-        <v>44</v>
-      </c>
       <c r="C3" s="9" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="42" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="28.2" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="B4" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="E4" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="28.2" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="D4" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="E4" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="42" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>50</v>
-      </c>
       <c r="E5" s="11" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -1911,8 +1903,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1A42715-6DB5-4D44-8227-1BC083C77DCE}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1949,16 +1941,16 @@
         <v>20</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>21</v>
@@ -1966,19 +1958,19 @@
     </row>
     <row r="3" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>21</v>

</xml_diff>